<commit_message>
added new anstellungsverhältnis prof
</commit_message>
<xml_diff>
--- a/data-migration/xlsx_1900-/1909_Sommer.xlsx
+++ b/data-migration/xlsx_1900-/1909_Sommer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\TEMP REPOSITORY\VVZ 1833-2014\_XLSX_2024-05-22\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E4429D-BB89-4F3C-89D5-94F4F9275F82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B21A89-4EFF-4977-9EEE-8D1315940882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17880" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2826" uniqueCount="1209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2826" uniqueCount="1210">
   <si>
     <t>1909</t>
   </si>
@@ -3660,6 +3660,9 @@
   </si>
   <si>
     <t>sidlerhuguenin_e</t>
+  </si>
+  <si>
+    <t>Prof</t>
   </si>
 </sst>
 </file>
@@ -4003,8 +4006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N398"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A376" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="H168" sqref="H168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8246,7 +8249,7 @@
         <v>1096</v>
       </c>
       <c r="I161" t="s">
-        <v>1179</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.25">
@@ -8272,7 +8275,7 @@
         <v>1096</v>
       </c>
       <c r="I162" t="s">
-        <v>1179</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.25">
@@ -8298,7 +8301,7 @@
         <v>1097</v>
       </c>
       <c r="I163" t="s">
-        <v>1179</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.25">
@@ -8324,7 +8327,7 @@
         <v>1097</v>
       </c>
       <c r="I164" t="s">
-        <v>1179</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.25">
@@ -8350,7 +8353,7 @@
         <v>1097</v>
       </c>
       <c r="I165" t="s">
-        <v>1179</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.25">
@@ -8376,7 +8379,7 @@
         <v>1097</v>
       </c>
       <c r="I166" t="s">
-        <v>1179</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.25">
@@ -8402,7 +8405,7 @@
         <v>1193</v>
       </c>
       <c r="I167" t="s">
-        <v>1179</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.25">
@@ -8428,7 +8431,7 @@
         <v>1193</v>
       </c>
       <c r="I168" t="s">
-        <v>1179</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>